<commit_message>
Added generic methods to read common data properties, read and write data into excel file
</commit_message>
<xml_diff>
--- a/data/testscript.xlsx
+++ b/data/testscript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sagar\eclipse-workspace\Automation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68A0108-0092-4F05-A09B-6742AF6D3306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8206D825-5D59-4133-AEB1-7C0D8FB7D7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{457AAEAF-74AA-4C84-8879-7672C920601C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{457AAEAF-74AA-4C84-8879-7672C920601C}"/>
   </bookViews>
   <sheets>
     <sheet name="createUser" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
   <si>
     <t>Sl no</t>
   </si>
@@ -62,9 +62,6 @@
     <t>sagar@gmail.com</t>
   </si>
   <si>
-    <t>sagardambal</t>
-  </si>
-  <si>
     <t>Item Name</t>
   </si>
   <si>
@@ -171,13 +168,18 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Samsung galaxy s25 ultra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,51 +579,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A723D443-F0E7-4A11-A100-F7CDA3F05F86}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.6640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.33203125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0">
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
         <v>9876543210</v>
       </c>
     </row>
@@ -643,197 +645,197 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.109375"/>
-    <col min="2" max="2" customWidth="true" width="13.33203125"/>
-    <col min="3" max="3" customWidth="true" width="11.88671875"/>
-    <col min="4" max="4" customWidth="true" width="11.77734375"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -845,121 +847,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CD08CE-34FF-4BE7-B73C-C044620D669F}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.109375"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s" s="0">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s" s="0">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>43</v>
+      <c r="C10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>